<commit_message>
Adding new admin interface
</commit_message>
<xml_diff>
--- a/api/routes/testSheet.xlsx
+++ b/api/routes/testSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\Popple\api\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83A8155-4385-4AE5-9AAA-1AED1F8D1000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CCA945-B1B1-49BE-B8A1-8C8C11411E30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C746189F-ED65-49FA-B73F-90D6F8A02364}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>CSC110</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>requirements</t>
+  </si>
+  <si>
+    <t>CSC335</t>
+  </si>
+  <si>
+    <t>CSC372</t>
+  </si>
+  <si>
+    <t>CSC473</t>
+  </si>
+  <si>
+    <t>CSC452</t>
+  </si>
+  <si>
+    <t>CSC345, CSC252, CSC352</t>
+  </si>
+  <si>
+    <t>CHEM</t>
   </si>
 </sst>
 </file>
@@ -418,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33E81A1-27C2-4BAA-8146-B315CDC8CE90}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +543,55 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>